<commit_message>
modif de normalize, enrich et excel_to_json
</commit_message>
<xml_diff>
--- a/work/normalized.xlsx
+++ b/work/normalized.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,22 +483,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Springsteen : Deliver me from nowhere</t>
+          <t>Mektoub my love Canto due</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>VO</t>
+          <t>VF</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -507,90 +507,90 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Découverte</t>
+          <t>Coup de cœur</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Les aigles de la république VO</t>
+          <t>La bonne étoile</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>VO</t>
+          <t>VF</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Coup de coeur</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Séance EPHAD HANDI - Famille</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>TU 5 €</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Classe moyenne</t>
+          <t>Eleanor the great</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Séance EPHAD HANDI</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>TU 5 €</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Découverte</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Kaamelott 2e volet - partie 1</t>
+          <t>La petite fanfare de Noël</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -600,94 +600,94 @@
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>JP</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>TU 3 €</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sam le pompier - nouvelles casernes, grandes aventures ! JP TU 3 €</t>
+          <t>Gatsby le magnifique</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>JP TU 3 €</t>
-        </is>
-      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ciné Patrimoine du samedi 18h</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>ADH 4 € - Autres 5 €</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Sacré Cœur</t>
+          <t>L'intermédiaire (Relay)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Ciné Documentaire du samedi 18h</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>ADH 4 € - Autres 5 €</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>DOC - partenariat paroisse</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>L'étranger</t>
+          <t>Zootopie 2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -697,28 +697,28 @@
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>JP</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Coup de coeur</t>
-        </is>
-      </c>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Invisibles mais infiniment précieux</t>
+          <t>La condition</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -729,31 +729,27 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>TU 5 €</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
-          <t>DOC + réalisateur invité et échange  ; DCP St Gaudens</t>
+          <t>Coup de cœur</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Six jours ce printemps-là</t>
+          <t>Mission Père Noël</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -763,18 +759,18 @@
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>JP</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>RG</t>
-        </is>
-      </c>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -784,12 +780,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Lumière pâle sur les collines</t>
+          <t>Kika</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>VO</t>
+          <t>VF</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -805,17 +801,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Film Mission locale - restitution travail d'atelier</t>
+          <t>Marcel et Monsieur Pagnol</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -824,23 +820,19 @@
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Séance avec la Mission locale - projection par ordi</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>JP</t>
+        </is>
+      </c>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>ouvert au public - gratuit - pas de pasage par Cinéfol</t>
-        </is>
-      </c>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -850,12 +842,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>T'as pas changé</t>
+          <t>Bugonia</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -867,17 +859,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>15:30</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Le secret des mésanges</t>
+          <t>Zootopie 2</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -889,42 +881,38 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Ciné goûter</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>JP</t>
-        </is>
-      </c>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Une bataille après l'autre</t>
+          <t>Le chant des forêts</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>VO</t>
+          <t>VF</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Ciné Jeunes du samedi 18h</t>
+          <t>Ciné Documentaire du samedi 18h</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -932,16 +920,12 @@
           <t>ADH 4 € - Autres 5 €</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Coup de coeur</t>
-        </is>
-      </c>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -951,7 +935,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Yoroï</t>
+          <t>On vous croit</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -963,12 +947,16 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Coup de cœur</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -978,7 +966,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Arco</t>
+          <t>Panique à Noël</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -988,18 +976,22 @@
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>JP TU 4,50 €</t>
-        </is>
-      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>JP</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>TU 4,50 €</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1009,7 +1001,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Dossier 137</t>
+          <t>Les enfants vont bien</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1026,77 +1018,69 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>L'amour qu'il nous reste</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>VF</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2 avant-premières uniquement sur invitation - TU 5 € - payé par le distributeur,</t>
-        </is>
-      </c>
+          <t>VO</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>CM1</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>DOC - ne pas mettre dans programme</t>
-        </is>
-      </c>
+      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Duel à Monte Carlo del norte</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Jour2Fête - en présencecdu réalisateur Edouard Bergeon et de Jérome Bayle</t>
-        </is>
-      </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
-          <t>DOC - ne pas mettre dans programme</t>
+          <t>Animé adulte - Découverte</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1106,12 +1090,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Des preuves d'amour</t>
+          <t>Reedland</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -1120,14 +1104,14 @@
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Coup de cœur</t>
+          <t>Découverte</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1137,7 +1121,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Egoist</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1149,74 +1133,78 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>Découverte</t>
-        </is>
-      </c>
+      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>La voix de Hind Rajab</t>
+          <t>Premières neiges</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>VO</t>
+          <t>VF</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Ciné goûter JP</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>TU 3 €</t>
+        </is>
+      </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Coup de cœur</t>
+          <t>3h02</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Salle non dispo de 14h à 19h</t>
+          <t>Apocalypse now final cut</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Séance EPHAD HANDI</t>
+          <t>Ciné Jeunes du samedi 18h</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>TU 5 €</t>
+          <t>ADH 4 € - Autres 5 €</t>
         </is>
       </c>
       <c r="I24" t="inlineStr"/>
@@ -1224,7 +1212,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1234,7 +1222,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>La femme la plus riche du monde</t>
+          <t>Louise</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1246,26 +1234,22 @@
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>repas école</t>
-        </is>
-      </c>
+      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>L'incroyable femme des neiges</t>
+          <t>A la poursuite du Père Noël</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1275,55 +1259,63 @@
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>JP Famille</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Détective Conan : La mémoire retrouvée JP</t>
+          <t>L'agent secret</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Prix mise en scène et interprétation masculine Cannes 2025</t>
+        </is>
+      </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>2h40 - Coup de cœur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Vie privée</t>
+          <t>L'âme idéale</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1331,43 +1323,55 @@
           <t>VF</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>CM2</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Découverte</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Les braises</t>
+          <t>Le maitre du Kabuki</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2h54 - Découverte</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1377,7 +1381,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Dites-lui que je l'aime</t>
+          <t>Animal totem</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1385,61 +1389,65 @@
           <t>VF</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>CM1</t>
+        </is>
+      </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>Découverte</t>
-        </is>
-      </c>
+      <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Un poète</t>
+          <t>Chasse gardée 2</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>VO</t>
+          <t>VF</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>Coup de cœur</t>
-        </is>
-      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Séance EPHAD HANDI</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>TU 5 €</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>T'as pas changé</t>
+          <t>Sacré Cœur</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1451,7 +1459,7 @@
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Séance EPHAD HANDI</t>
+          <t>DOC</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1464,7 +1472,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1474,38 +1482,42 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>France, une histoire d'amour</t>
+          <t>Resurrection</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>VF</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Prix spécial Cannes 2025</t>
+        </is>
+      </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr">
         <is>
-          <t>DOC</t>
+          <t>2h40 - Coup de cœur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>15:30</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Thelma du pays des glaces</t>
+          <t>Le roi des rois</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1515,18 +1527,18 @@
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>JP</t>
+        </is>
+      </c>
       <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>JP</t>
-        </is>
-      </c>
+      <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1536,19 +1548,23 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Eve</t>
+          <t>L'engloutie</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>VO</t>
+          <t>VF</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Prix Jean Vigo 2025</t>
+        </is>
+      </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Ciné Patrimoine du samedi 18h</t>
+          <t>Ciné discussion</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1556,22 +1572,26 @@
           <t>ADH 4 € - Autres 5 €</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Coup de cœur</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Les rêveurs</t>
+          <t>Heidi et le lynx des montagnes</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1581,24 +1601,32 @@
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>JP</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>TU 4,50 €</t>
+        </is>
+      </c>
       <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Le secret des mésanges JP</t>
+          <t>Avatar De feu et de cendres</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1612,90 +1640,40 @@
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr">
         <is>
-          <t>JP TU 4,50 €</t>
+          <t>3h17 2D</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Jean Valjean</t>
+          <t>Fuori</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>VF</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr"/>
+          <t>VO</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>CM2</t>
+        </is>
+      </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>2025-12-23</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Wicked partie 2</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>VF</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>2025-12-23</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>21:00</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>La vague VO</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>VO</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr">
+      <c r="I38" t="inlineStr">
         <is>
           <t>Découverte</t>
         </is>

</xml_diff>